<commit_message>
Slope estimation of N170 values and implementation into mixed model to see if the slope has significant effect on N170 values (no effect). General variance estimation and visualisation of N170
</commit_message>
<xml_diff>
--- a/data/erp_N170_HC_and_MDD.xlsx
+++ b/data/erp_N170_HC_and_MDD.xlsx
@@ -409,6 +409,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -465,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -484,6 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -764,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H643"/>
+  <dimension ref="A1:I643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,9 +783,10 @@
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -807,7 +812,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -832,8 +837,9 @@
       <c r="H2" s="4">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -859,7 +865,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -885,7 +891,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -911,7 +917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -937,7 +943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -963,7 +969,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -989,7 +995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1014,8 +1020,9 @@
       <c r="H9" s="4">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1041,7 +1048,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1067,7 +1074,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1093,7 +1100,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1119,7 +1126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -1144,8 +1151,9 @@
       <c r="H14" s="4">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1171,7 +1179,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -1197,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -1223,7 +1231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -1249,7 +1257,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1275,7 +1283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -1300,8 +1308,9 @@
       <c r="H20" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -1327,7 +1336,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1353,7 +1362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -1379,7 +1388,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -1405,7 +1414,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -1431,7 +1440,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1456,8 +1465,9 @@
       <c r="H26" s="4">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1483,7 +1493,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -1509,7 +1519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -1535,7 +1545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -1561,7 +1571,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -1587,7 +1597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>